<commit_message>
description sur 3 lignes
</commit_message>
<xml_diff>
--- a/mecaniscout.xlsx
+++ b/mecaniscout.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="220">
   <si>
     <t xml:space="preserve">Type</t>
   </si>
@@ -46,16 +46,16 @@
     <t xml:space="preserve">Competence</t>
   </si>
   <si>
-    <t xml:space="preserve">speedometer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rapidité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">walking-boot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endurance</t>
+    <t xml:space="preserve">strong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effort physique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utiliser sa force, sa rapidité, son endurance pour réaliser une action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je me lance à fond dans une course de relai</t>
   </si>
   <si>
     <t xml:space="preserve">bullseye</t>
@@ -64,7 +64,10 @@
     <t xml:space="preserve">Dextérité</t>
   </si>
   <si>
-    <t xml:space="preserve">Viser, lancer, attraper</t>
+    <t xml:space="preserve">Utiliser ses capacités à viser, lancer, attraper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai envoyé ma flèche polynésienne pile au centre de la cible !</t>
   </si>
   <si>
     <t xml:space="preserve">human-pyramid</t>
@@ -73,82 +76,130 @@
     <t xml:space="preserve">Coordination d'équipe</t>
   </si>
   <si>
+    <t xml:space="preserve">Capacité à communiquer et prendre des décisions en équipe.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passez par la forêt, nous on passe par la plaine et on les prend en étau.</t>
+  </si>
+  <si>
     <t xml:space="preserve">light-bulb</t>
   </si>
   <si>
     <t xml:space="preserve">Stratégie</t>
   </si>
   <si>
+    <t xml:space="preserve">Savoir adapter sa manière de jouer au fonctionnement du jeu pour augmenter ses chances de gagner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C'est trop risqué d'attaquer Eulalie, je crois qu'elle est caporale.</t>
+  </si>
+  <si>
     <t xml:space="preserve">sly</t>
   </si>
   <si>
     <t xml:space="preserve">Ruse</t>
   </si>
   <si>
-    <t xml:space="preserve">Bluffer, contourner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">disc</t>
+    <t xml:space="preserve">Capacité à utiliser des procédé habile pour tromper, dissimuler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viens m'attraper, j'ai plein d'or, ou peut-être pas...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brain</t>
   </si>
   <si>
     <t xml:space="preserve">Mémorisation </t>
   </si>
   <si>
+    <t xml:space="preserve">Retenir des éléments utile pour la suite du jeu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À cet endroit, il y avait une brosse à dent !</t>
+  </si>
+  <si>
     <t xml:space="preserve">wax-tablet</t>
   </si>
   <si>
     <t xml:space="preserve">Décodage</t>
   </si>
   <si>
+    <t xml:space="preserve">Connaître des codes ou savoir utiliser un outil de décodage pour déchiffrer un message.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je reconnais, c'est codé en K6 !</t>
+  </si>
+  <si>
     <t xml:space="preserve">treasure-map</t>
   </si>
   <si>
     <t xml:space="preserve">Lecture de carte</t>
   </si>
   <si>
+    <t xml:space="preserve">Repérer les routes, les éléments géographique, connaître le dénivelé en regardant une carte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Après la 4ème rue, on tombera sur un chateau d'eau</t>
+  </si>
+  <si>
     <t xml:space="preserve">gift-of-knowledge</t>
   </si>
   <si>
     <t xml:space="preserve">Connaissance</t>
   </si>
   <si>
+    <t xml:space="preserve">Restitution d'informations sur des sujets hors du jeu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baden-Powell est né un 22 février.</t>
+  </si>
+  <si>
     <t xml:space="preserve">observatory</t>
   </si>
   <si>
     <t xml:space="preserve">Observation</t>
   </si>
   <si>
+    <t xml:space="preserve">Identification dans l'espace de divers éléments, plus ou moins dissimulés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regarde, au dessus du mur, il y a une gommette bleu, c'est l'indice qu'on cherchait !</t>
+  </si>
+  <si>
     <t xml:space="preserve">direction-signs</t>
   </si>
   <si>
     <t xml:space="preserve">Orientation</t>
   </si>
   <si>
-    <t xml:space="preserve">gears</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logique</t>
+    <t xml:space="preserve">Se repérer dans l'espace, savoir utiliser une bousole ou d'autres moyen de s'orienter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On a tourné 3 fois à gauche, on doit pas être loin du village maintenant</t>
   </si>
   <si>
     <t xml:space="preserve">inspiration</t>
   </si>
   <si>
-    <t xml:space="preserve">Esprit d'analyse / synthèse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">magnifying-glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fouille</t>
+    <t xml:space="preserve">Analyse - Synthèse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discerner des informations et éléments, les réunir pour établir une déduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La sorcière a utilisé sa potion pour ressuciter Samara, donc c'est Eulalie.</t>
   </si>
   <si>
     <t xml:space="preserve">hammer-nails</t>
   </si>
   <si>
-    <t xml:space="preserve">Manuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activités manuelles</t>
+    <t xml:space="preserve">Manuel - Artistique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacité à réaliser des tâches manuelles et artistiques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ton dessin d'hippopotame est vachement réussi. Euh... C'était un éléphant.</t>
   </si>
   <si>
     <t xml:space="preserve">body-balance</t>
@@ -157,6 +208,12 @@
     <t xml:space="preserve">Aisance corporelle</t>
   </si>
   <si>
+    <t xml:space="preserve">Être à l'aise avec son corps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quand j'aurais fini de faire la roue, on pour se mettre en équilibres sur la perche</t>
+  </si>
+  <si>
     <t xml:space="preserve">Materiel</t>
   </si>
   <si>
@@ -166,6 +223,9 @@
     <t xml:space="preserve">Balle</t>
   </si>
   <si>
+    <t xml:space="preserve">Petite sphère, boule élastique dont on se sert pour divers jeux.</t>
+  </si>
+  <si>
     <t xml:space="preserve">tennis-racket</t>
   </si>
   <si>
@@ -193,27 +253,27 @@
     <t xml:space="preserve">Permet de prendre la vie du joueur / De marquer qu'il est vivant</t>
   </si>
   <si>
+    <t xml:space="preserve">three-friends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marqueur d'équipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maquilage, morceau de tissus, etc. Qui permette de savoir l'équipe d'un joueur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id-card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marqueur d'identité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan / Carte géographique</t>
+  </si>
+  <si>
     <t xml:space="preserve">À clarifier</t>
   </si>
   <si>
-    <t xml:space="preserve">three-friends</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marqueur d'équipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maquilage, morceau de tissus, etc. Qui permette de savoir l'équipe d'un joueur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id-card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marqueur d'identité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan / Carte géographique</t>
-  </si>
-  <si>
     <t xml:space="preserve">pencil-brush</t>
   </si>
   <si>
@@ -274,7 +334,7 @@
     <t xml:space="preserve">Déguisement / Habilement</t>
   </si>
   <si>
-    <t xml:space="preserve">Rolling-dices</t>
+    <t xml:space="preserve">rolling-dices</t>
   </si>
   <si>
     <t xml:space="preserve">Dés</t>
@@ -343,42 +403,42 @@
     <t xml:space="preserve">123 soleil / teque</t>
   </si>
   <si>
+    <t xml:space="preserve">pentarrows-tornado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renversement / Bifurcation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evénement qui bouleverse le fonctionnement du jeu lorsqu'il se produit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gober à la teque, Jeu dont vous êtes le heros, attraper le vif d'or, taper dans le ballon à la gamelle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evoluer entre des espaces où s'appliquent des règles spécifiques.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parcours du combattant, balle aux prisonnier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">house</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Être en lieu sûr pour préparer sa stratégie, stocker ou cacher des éléments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prise de drapeau, Douanier-Contrebandier</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prise de risque</t>
   </si>
   <si>
-    <t xml:space="preserve">pentarrows-tornado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renversement / Bifurcation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evénement qui bouleverse le fonctionnement du jeu lorsqu'il se produit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gober à la teque, Jeu dont vous êtes le heros, attraper le vif d'or, taper dans le ballon à la gamelle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evoluer entre des espaces où s'appliquent des règles spécifiques.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parcours du combattant, balle aux prisonnier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">house</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Être en lieu sûr pour préparer sa stratégie, stocker ou cacher des éléments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prise de drapeau, Douanier-Contrebandier</t>
-  </si>
-  <si>
     <t xml:space="preserve">path-distance</t>
   </si>
   <si>
@@ -391,7 +451,7 @@
     <t xml:space="preserve">Parcours du combattant, teques</t>
   </si>
   <si>
-    <t xml:space="preserve">Network-bars</t>
+    <t xml:space="preserve">network-bars</t>
   </si>
   <si>
     <t xml:space="preserve">Progression</t>
@@ -442,57 +502,57 @@
     <t xml:space="preserve">Individuellement ou en équipe, des joueurs mettent en commun leurs efforts et ressource pour atteindre un objectif mutuel.</t>
   </si>
   <si>
+    <t xml:space="preserve">spy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identité secrete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cacher une partie de son identité aux autres joueurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organigram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiérarchie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relation de force faiblesse entre joueurs / équipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poule, Renard, Vipère, Zagamore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swords-power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confrontation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Résoudre une situation de jeu ponctuelle opposant directement plusieurs joueurs ou équipes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Formel / informel, équilibré / déséquilibré</t>
   </si>
   <si>
-    <t xml:space="preserve">spy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identité secrete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cacher une partie de son identité aux autres joueurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">organigram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hiérarchie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relation de force faiblesse entre joueurs / équipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poule, Renard, Vipère, Zagamore</t>
+    <t xml:space="preserve">Récuperation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Récupérer des objets à l'ennemi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informations cachées</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cacher ou dissimuler aux joueurs des informations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Message codé, Élement omis dans une histoire, Physiquement</t>
   </si>
   <si>
     <t xml:space="preserve">À reformuler</t>
   </si>
   <si>
-    <t xml:space="preserve">swords-power</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Confrontation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Résoudre une situation de jeu ponctuelle opposant directement plusieurs joueurs ou équipes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Récuperation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Récupérer des objets à l'ennemi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Informations cachées</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cacher ou dissimuler aux joueurs des informations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Message codé, Élement omis dans une histoire, Physiquement</t>
-  </si>
-  <si>
     <t xml:space="preserve">gamepad</t>
   </si>
   <si>
@@ -589,22 +649,22 @@
     <t xml:space="preserve">Amphithéatre</t>
   </si>
   <si>
+    <t xml:space="preserve">forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forêt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À cachette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eclipse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sombre</t>
+  </si>
+  <si>
     <t xml:space="preserve">Trouver plus général</t>
-  </si>
-  <si>
-    <t xml:space="preserve">forest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forêt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À cachette</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eclipse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sombre</t>
   </si>
   <si>
     <t xml:space="preserve">talk</t>
@@ -740,11 +800,11 @@
   </sheetPr>
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -769,7 +829,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -779,249 +839,301 @@
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="F5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="F6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="F7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="F8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="F11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+        <v>49</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="F12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="F13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+        <v>57</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="F14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+        <v>61</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="E16" s="3"/>
       <c r="F16" s="1" t="n">
         <v>1</v>
@@ -1030,16 +1142,16 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="1" t="n">
@@ -1047,52 +1159,56 @@
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="3"/>
+        <v>72</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="E18" s="3"/>
       <c r="F18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="E19" s="3"/>
       <c r="F19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="1" t="n">
@@ -1100,74 +1216,68 @@
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>60</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1176,15 +1286,15 @@
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1193,15 +1303,15 @@
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1210,17 +1320,19 @@
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D27" s="3"/>
+        <v>91</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="E27" s="3"/>
       <c r="F27" s="1" t="n">
         <v>1</v>
@@ -1229,13 +1341,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1244,15 +1356,15 @@
       </c>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1261,18 +1373,18 @@
       </c>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="1" t="n">
@@ -1280,15 +1392,15 @@
       </c>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -1297,15 +1409,15 @@
       </c>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -1314,51 +1426,51 @@
       </c>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" s="3"/>
+        <v>107</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="E34" s="3"/>
       <c r="F34" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -1367,35 +1479,37 @@
       </c>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="3"/>
+        <v>112</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="E36" s="3"/>
       <c r="F36" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="1" t="n">
@@ -1405,13 +1519,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -1420,19 +1534,17 @@
       </c>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>93</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="1" t="n">
         <v>1</v>
@@ -1441,133 +1553,143 @@
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>45</v>
+        <v>123</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="F41" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>45</v>
+        <v>123</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="F42" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>123</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
+        <v>131</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="F43" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>51</v>
+        <v>134</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="F44" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="F45" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G45" s="4"/>
     </row>
-    <row r="46" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>51</v>
+        <v>143</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="F46" s="1" t="n">
         <v>1</v>
@@ -1576,98 +1698,92 @@
     </row>
     <row r="47" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="E47" s="3"/>
       <c r="F47" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G47" s="4"/>
     </row>
-    <row r="48" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>122</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="E48" s="3"/>
       <c r="F48" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G48" s="4"/>
     </row>
-    <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E49" s="3"/>
+      <c r="F49" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G49" s="4"/>
+    </row>
+    <row r="50" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F49" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G49" s="4"/>
-    </row>
-    <row r="50" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="B50" s="1" t="s">
-        <v>127</v>
+        <v>71</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="1" t="n">
@@ -1675,18 +1791,18 @@
       </c>
       <c r="G51" s="4"/>
     </row>
-    <row r="52" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>51</v>
+        <v>160</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="1" t="n">
@@ -1694,58 +1810,62 @@
       </c>
       <c r="G52" s="4"/>
     </row>
-    <row r="53" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>51</v>
+        <v>163</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E53" s="3"/>
+        <v>165</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="F53" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G53" s="4"/>
     </row>
-    <row r="54" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E54" s="3"/>
+        <v>169</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="F54" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>141</v>
+        <v>71</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="1" t="n">
@@ -1753,62 +1873,60 @@
       </c>
       <c r="G55" s="4"/>
     </row>
-    <row r="56" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>144</v>
+        <v>71</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="F56" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>150</v>
+        <v>178</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>147</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="E57" s="3"/>
       <c r="F57" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G57" s="4"/>
     </row>
-    <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="1" t="n">
@@ -1816,93 +1934,85 @@
       </c>
       <c r="G58" s="4"/>
     </row>
-    <row r="59" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>156</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="E59" s="3"/>
       <c r="F59" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G59" s="4"/>
     </row>
-    <row r="60" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>103</v>
+        <v>184</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>159</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G60" s="4"/>
     </row>
-    <row r="61" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>103</v>
+        <v>184</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>51</v>
+        <v>187</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>161</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G61" s="4"/>
     </row>
-    <row r="62" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>103</v>
+        <v>184</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>51</v>
+        <v>189</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>163</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G62" s="4"/>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>165</v>
+        <v>71</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>166</v>
+        <v>191</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -1911,15 +2021,15 @@
       </c>
       <c r="G63" s="4"/>
     </row>
-    <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -1928,15 +2038,15 @@
       </c>
       <c r="G64" s="4"/>
     </row>
-    <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -1945,15 +2055,15 @@
       </c>
       <c r="G65" s="4"/>
     </row>
-    <row r="66" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>51</v>
+        <v>196</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -1962,15 +2072,15 @@
       </c>
       <c r="G66" s="4"/>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>172</v>
+        <v>71</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -1981,13 +2091,13 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>164</v>
+        <v>199</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
@@ -1996,32 +2106,34 @@
       </c>
       <c r="G68" s="4"/>
     </row>
-    <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>164</v>
+        <v>199</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D69" s="3"/>
+        <v>203</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="E69" s="3"/>
       <c r="F69" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G69" s="4"/>
     </row>
-    <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>164</v>
+        <v>199</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>51</v>
+        <v>205</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
@@ -2030,15 +2142,15 @@
       </c>
       <c r="G70" s="4"/>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>180</v>
+        <v>207</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>181</v>
+        <v>208</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
@@ -2047,34 +2159,32 @@
       </c>
       <c r="G71" s="4"/>
     </row>
-    <row r="72" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>184</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G72" s="4"/>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>185</v>
+        <v>71</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
@@ -2085,13 +2195,13 @@
     </row>
     <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
@@ -2099,37 +2209,41 @@
         <v>1</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>179</v>
+        <v>7</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>190</v>
+        <v>215</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D75" s="3"/>
+        <v>216</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="E75" s="3"/>
       <c r="F75" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G75" s="4"/>
     </row>
-    <row r="76" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>179</v>
+        <v>7</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>51</v>
+        <v>157</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D76" s="3"/>
+        <v>218</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="E76" s="3"/>
       <c r="F76" s="1" t="n">
         <v>1</v>
@@ -2138,13 +2252,13 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>193</v>
+        <v>212</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
@@ -2158,13 +2272,13 @@
         <v>7</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="E78" s="3"/>
       <c r="F78" s="1" t="n">
@@ -2177,13 +2291,13 @@
         <v>7</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="1" t="n">

</xml_diff>